<commit_message>
add calculation time count
</commit_message>
<xml_diff>
--- a/results_Potential_NextBlock.xlsx
+++ b/results_Potential_NextBlock.xlsx
@@ -36,11 +36,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000000FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
@@ -52,6 +47,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000000FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -123,16 +123,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -560,7 +560,7 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="E1" s="1" t="n">
@@ -568,36 +568,31 @@
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="G1" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="I1" s="3" t="n">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="K1" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="M1" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="O1" s="3" t="n">
         <v>7</v>
       </c>
@@ -620,12 +615,22 @@
       <c r="U1" s="6" t="n">
         <v>10</v>
       </c>
+      <c r="V1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="W1" s="6" t="n">
         <v>11</v>
       </c>
       <c r="Y1" s="7" t="n">
         <v>12</v>
       </c>
+      <c r="Z1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="AA1" s="7" t="n">
         <v>13</v>
       </c>
@@ -636,6 +641,11 @@
       </c>
       <c r="AC1" s="7" t="n">
         <v>14</v>
+      </c>
+      <c r="AD1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
       <c r="AE1" s="7" t="n">
         <v>15</v>
@@ -654,22 +664,17 @@
     <row r="2" ht="20" customHeight="1">
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
       <c r="M2" s="2" t="inlineStr">
         <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
+          <t>↑</t>
         </is>
       </c>
       <c r="Q2" s="2" t="inlineStr">
@@ -682,14 +687,9 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="W2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
       <c r="Y2" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
+          <t>↓</t>
         </is>
       </c>
       <c r="AA2" s="2" t="inlineStr">
@@ -697,9 +697,9 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="AE2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
+      <c r="AC2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
         </is>
       </c>
       <c r="AG2" s="8" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="AH2" s="2" t="inlineStr">
         <is>
-          <t>4 → 9</t>
+          <t>2 → 6</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
@@ -728,53 +728,58 @@
       <c r="E3" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="G3" s="1" t="n">
         <v>19</v>
       </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="I3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="K3" s="3" t="n">
         <v>21</v>
       </c>
       <c r="M3" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="O3" s="3" t="n">
         <v>23</v>
       </c>
       <c r="Q3" s="6" t="n">
         <v>24</v>
       </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="S3" s="6" t="n">
         <v>25</v>
       </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="U3" s="6" t="n">
         <v>26</v>
       </c>
       <c r="V3" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="W3" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="X3" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="Y3" s="7" t="n">
         <v>28</v>
       </c>
@@ -786,7 +791,7 @@
       </c>
       <c r="AD3" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="AE3" s="7" t="n">
@@ -799,14 +804,14 @@
       </c>
       <c r="AH3" s="2" t="inlineStr">
         <is>
-          <t>3 → 9</t>
+          <t>0 → 7</t>
         </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -814,9 +819,19 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="O4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
       <c r="Q4" s="2" t="inlineStr">
@@ -824,11 +839,6 @@
           <t>↓</t>
         </is>
       </c>
-      <c r="S4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
       <c r="U4" s="2" t="inlineStr">
         <is>
           <t>↓</t>
@@ -836,7 +846,7 @@
       </c>
       <c r="W4" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
+          <t>↓</t>
         </is>
       </c>
       <c r="AA4" s="2" t="inlineStr">
@@ -844,14 +854,9 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="AC4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
       <c r="AE4" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
+          <t>↓</t>
         </is>
       </c>
       <c r="AG4" s="10" t="inlineStr">
@@ -861,7 +866,7 @@
       </c>
       <c r="AH4" s="2" t="inlineStr">
         <is>
-          <t>2 → 9</t>
+          <t>0 → 9</t>
         </is>
       </c>
     </row>
@@ -879,17 +884,12 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="E5" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="G5" s="1" t="n">
         <v>35</v>
       </c>
@@ -925,6 +925,11 @@
       <c r="O5" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="Q5" s="6" t="n">
         <v>40</v>
       </c>
@@ -947,17 +952,12 @@
       </c>
       <c r="Z5" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="AA5" s="7" t="n">
         <v>45</v>
       </c>
-      <c r="AB5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="AC5" s="7" t="n">
         <v>46</v>
       </c>
@@ -971,7 +971,7 @@
       </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
-          <t>4 → 6</t>
+          <t>0 → 7</t>
         </is>
       </c>
     </row>
@@ -981,11 +981,6 @@
           <t>↓</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
           <t>↓</t>
@@ -996,27 +991,27 @@
           <t>↓</t>
         </is>
       </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
       <c r="Q6" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="W6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AE6" s="2" t="inlineStr">
+      <c r="U6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="Y6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AA6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="AC6" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
@@ -1028,7 +1023,7 @@
       </c>
       <c r="AH6" s="2" t="inlineStr">
         <is>
-          <t>1 → 9</t>
+          <t>2 → 9</t>
         </is>
       </c>
     </row>
@@ -1036,6 +1031,11 @@
       <c r="A7" s="1" t="n">
         <v>48</v>
       </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="n">
         <v>49</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="K7" s="3" t="n">
@@ -1058,29 +1058,34 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="M7" s="3" t="n">
         <v>54</v>
       </c>
+      <c r="N7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="O7" s="3" t="n">
         <v>55</v>
       </c>
+      <c r="P7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="Q7" s="6" t="n">
         <v>56</v>
       </c>
-      <c r="R7" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="S7" s="6" t="n">
         <v>57</v>
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="U7" s="6" t="n">
@@ -1101,11 +1106,6 @@
       </c>
       <c r="Y7" s="7" t="n">
         <v>60</v>
-      </c>
-      <c r="Z7" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
       </c>
       <c r="AA7" s="7" t="n">
         <v>61</v>
@@ -1203,11 +1203,6 @@
       <c r="E1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="n">
         <v>3</v>
       </c>
@@ -1227,6 +1222,11 @@
       <c r="K1" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="M1" s="3" t="n">
         <v>6</v>
       </c>
@@ -1273,11 +1273,6 @@
       <c r="Y1" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="AA1" s="7" t="n">
         <v>13</v>
       </c>
@@ -1309,19 +1304,19 @@
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>↓</t>
+          <t>↑</t>
         </is>
       </c>
       <c r="O2" s="2" t="inlineStr">
@@ -1344,9 +1339,9 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="AE2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
+      <c r="AA2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
         </is>
       </c>
       <c r="AG2" s="8" t="inlineStr">
@@ -1356,7 +1351,7 @@
       </c>
       <c r="AH2" s="2" t="inlineStr">
         <is>
-          <t>4 → 9</t>
+          <t>2 → 6</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1361,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
@@ -1375,39 +1370,34 @@
       <c r="E3" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="G3" s="1" t="n">
         <v>19</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="K3" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="M3" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="O3" s="3" t="n">
         <v>23</v>
       </c>
       <c r="Q3" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="R3" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="S3" s="6" t="n">
         <v>25</v>
       </c>
@@ -1419,6 +1409,11 @@
       <c r="U3" s="6" t="n">
         <v>26</v>
       </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="W3" s="6" t="n">
         <v>27</v>
       </c>
@@ -1438,7 +1433,7 @@
       </c>
       <c r="AD3" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="AE3" s="7" t="n">
@@ -1451,14 +1446,14 @@
       </c>
       <c r="AH3" s="2" t="inlineStr">
         <is>
-          <t>3 → 9</t>
+          <t>0 → 7</t>
         </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -1468,11 +1463,6 @@
       </c>
       <c r="M4" s="2" t="inlineStr">
         <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="O4" s="2" t="inlineStr">
-        <is>
           <t>↑</t>
         </is>
       </c>
@@ -1483,27 +1473,22 @@
       </c>
       <c r="S4" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="U4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
+          <t>↓</t>
         </is>
       </c>
       <c r="W4" s="2" t="inlineStr">
         <is>
-          <t>↓</t>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="Y4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
       <c r="AC4" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AE4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
+          <t>↓</t>
         </is>
       </c>
       <c r="AG4" s="10" t="inlineStr">
@@ -1513,7 +1498,7 @@
       </c>
       <c r="AH4" s="2" t="inlineStr">
         <is>
-          <t>2 → 9</t>
+          <t>0 → 9</t>
         </is>
       </c>
     </row>
@@ -1521,27 +1506,12 @@
       <c r="A5" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="C5" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="E5" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="G5" s="1" t="n">
         <v>35</v>
       </c>
@@ -1550,7 +1520,7 @@
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="K5" s="3" t="n">
@@ -1559,28 +1529,33 @@
       <c r="M5" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="N5" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
       <c r="O5" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="Q5" s="6" t="n">
         <v>40</v>
       </c>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="S5" s="6" t="n">
         <v>41</v>
       </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="U5" s="6" t="n">
         <v>42</v>
       </c>
-      <c r="V5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="W5" s="6" t="n">
         <v>43</v>
       </c>
@@ -1595,9 +1570,19 @@
       <c r="AA5" s="7" t="n">
         <v>45</v>
       </c>
+      <c r="AB5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="AC5" s="7" t="n">
         <v>46</v>
       </c>
+      <c r="AD5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="AE5" s="7" t="n">
         <v>47</v>
       </c>
@@ -1608,22 +1593,37 @@
       </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
-          <t>4 → 6</t>
+          <t>0 → 7</t>
         </is>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="O6" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
@@ -1633,14 +1633,19 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="U6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="Y6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
+      <c r="W6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AA6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AC6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
       <c r="AG6" s="12" t="inlineStr">
@@ -1650,7 +1655,7 @@
       </c>
       <c r="AH6" s="2" t="inlineStr">
         <is>
-          <t>1 → 9</t>
+          <t>2 → 9</t>
         </is>
       </c>
     </row>
@@ -1660,7 +1665,7 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="C7" s="1" t="n">
@@ -1668,7 +1673,7 @@
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="E7" s="1" t="n">
@@ -1676,7 +1681,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="G7" s="1" t="n">
@@ -1684,7 +1689,7 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="I7" s="3" t="n">
@@ -1692,18 +1697,23 @@
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="K7" s="3" t="n">
         <v>53</v>
       </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="M7" s="3" t="n">
         <v>54</v>
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="O7" s="3" t="n">
@@ -1720,37 +1730,27 @@
       <c r="S7" s="6" t="n">
         <v>57</v>
       </c>
+      <c r="T7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="U7" s="6" t="n">
         <v>58</v>
       </c>
-      <c r="V7" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="W7" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="X7" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
       <c r="Y7" s="7" t="n">
         <v>60</v>
       </c>
       <c r="Z7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="AA7" s="7" t="n">
         <v>61</v>
-      </c>
-      <c r="AB7" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
       </c>
       <c r="AC7" s="7" t="n">
         <v>62</v>

</xml_diff>

<commit_message>
add new penalty(車の向き) and its weight
</commit_message>
<xml_diff>
--- a/results_Potential_NextBlock.xlsx
+++ b/results_Potential_NextBlock.xlsx
@@ -27,7 +27,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -36,12 +36,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFC0CB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0087CEEB"/>
+        <fgColor rgb="000000FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -51,7 +46,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000000FF"/>
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -61,12 +56,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FAEBD7"/>
+        <fgColor rgb="00FFC0CB"/>
       </patternFill>
     </fill>
   </fills>
@@ -110,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
@@ -121,31 +111,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -157,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,7 +503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,7 +579,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="I1" s="3" t="n">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="inlineStr">
@@ -609,7 +587,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="K1" s="4" t="n">
+      <c r="K1" s="3" t="n">
         <v>5</v>
       </c>
       <c r="L1" s="2" t="inlineStr">
@@ -617,7 +595,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="M1" s="4" t="n">
+      <c r="M1" s="3" t="n">
         <v>6</v>
       </c>
       <c r="N1" s="2" t="inlineStr">
@@ -625,7 +603,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="O1" s="4" t="n">
+      <c r="O1" s="3" t="n">
         <v>7</v>
       </c>
       <c r="P1" s="2" t="inlineStr">
@@ -633,7 +611,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="n">
+      <c r="Q1" s="4" t="n">
         <v>8</v>
       </c>
       <c r="R1" s="2" t="inlineStr">
@@ -641,13 +619,18 @@
           <t>→</t>
         </is>
       </c>
-      <c r="S1" s="6" t="n">
+      <c r="S1" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="U1" s="7" t="n">
+      <c r="U1" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="W1" s="7" t="n">
+      <c r="V1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="W1" s="6" t="n">
         <v>11</v>
       </c>
       <c r="X1" s="2" t="inlineStr">
@@ -655,7 +638,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Y1" s="3" t="n">
+      <c r="Y1" s="6" t="n">
         <v>12</v>
       </c>
       <c r="Z1" s="2" t="inlineStr">
@@ -663,10 +646,15 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AA1" s="3" t="n">
+      <c r="AA1" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="AC1" s="3" t="n">
+      <c r="AB1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AC1" s="6" t="n">
         <v>14</v>
       </c>
       <c r="AD1" s="2" t="inlineStr">
@@ -674,7 +662,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AE1" s="3" t="n">
+      <c r="AE1" s="6" t="n">
         <v>15</v>
       </c>
       <c r="AG1" s="2" t="inlineStr">
@@ -689,69 +677,29 @@
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="E2" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="Q2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="U2" s="2" t="inlineStr">
+      <c r="W2" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="W2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AA2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AC2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AG2" s="8" t="inlineStr">
+      <c r="AG2" s="7" t="inlineStr">
         <is>
           <t>car 0</t>
         </is>
       </c>
       <c r="AH2" s="2" t="inlineStr">
         <is>
-          <t>0 → 5</t>
+          <t>3 → 5</t>
         </is>
       </c>
     </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="8" t="n">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -759,7 +707,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="8" t="n">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -767,10 +715,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="n">
         <v>19</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -778,19 +731,39 @@
           <t>←</t>
         </is>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O3" s="4" t="n">
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="O3" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q3" s="7" t="n">
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="Q3" s="3" t="n">
         <v>24</v>
       </c>
       <c r="R3" s="2" t="inlineStr">
@@ -798,7 +771,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="S3" s="7" t="n">
+      <c r="S3" s="3" t="n">
         <v>25</v>
       </c>
       <c r="T3" s="2" t="inlineStr">
@@ -806,7 +779,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="6" t="n">
         <v>26</v>
       </c>
       <c r="V3" s="2" t="inlineStr">
@@ -814,18 +787,23 @@
           <t>→</t>
         </is>
       </c>
-      <c r="W3" s="7" t="n">
+      <c r="W3" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="Y3" s="3" t="n">
+      <c r="X3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="Y3" s="6" t="n">
         <v>28</v>
       </c>
       <c r="Z3" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="AA3" s="3" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AA3" s="6" t="n">
         <v>29</v>
       </c>
       <c r="AB3" s="2" t="inlineStr">
@@ -833,7 +811,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AC3" s="3" t="n">
+      <c r="AC3" s="6" t="n">
         <v>30</v>
       </c>
       <c r="AD3" s="2" t="inlineStr">
@@ -841,64 +819,39 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AE3" s="3" t="n">
+      <c r="AE3" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="AG3" s="10" t="inlineStr">
+      <c r="AG3" s="9" t="inlineStr">
         <is>
           <t>car 1</t>
         </is>
       </c>
       <c r="AH3" s="2" t="inlineStr">
         <is>
-          <t>1 → 6</t>
+          <t>0 → 9</t>
         </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="E4" s="2" t="inlineStr">
+      <c r="S4" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="Q4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="S4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="U4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AG4" s="11" t="inlineStr">
+      <c r="AG4" s="10" t="inlineStr">
         <is>
           <t>car 2</t>
         </is>
       </c>
       <c r="AH4" s="2" t="inlineStr">
         <is>
-          <t>4 → 6</t>
+          <t>0 → 7</t>
         </is>
       </c>
     </row>
     <row r="5" ht="50" customHeight="1">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="8" t="n">
         <v>32</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -906,16 +859,31 @@
           <t>←</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="8" t="n">
         <v>33</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="n">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -923,27 +891,47 @@
           <t>←</t>
         </is>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="K5" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="n">
         <v>38</v>
       </c>
       <c r="N5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="O5" s="12" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="O5" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="Q5" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="S5" s="12" t="n">
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="S5" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="U5" s="6" t="n">
         <v>42</v>
       </c>
       <c r="V5" s="2" t="inlineStr">
@@ -951,7 +939,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="W5" s="7" t="n">
+      <c r="W5" s="6" t="n">
         <v>43</v>
       </c>
       <c r="X5" s="2" t="inlineStr">
@@ -959,7 +947,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Y5" s="3" t="n">
+      <c r="Y5" s="6" t="n">
         <v>44</v>
       </c>
       <c r="Z5" s="2" t="inlineStr">
@@ -967,7 +955,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AA5" s="3" t="n">
+      <c r="AA5" s="6" t="n">
         <v>45</v>
       </c>
       <c r="AB5" s="2" t="inlineStr">
@@ -975,90 +963,55 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AC5" s="3" t="n">
+      <c r="AC5" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="AE5" s="3" t="n">
+      <c r="AD5" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AE5" s="6" t="n">
         <v>47</v>
       </c>
-      <c r="AG5" s="13" t="inlineStr">
+      <c r="AG5" s="11" t="inlineStr">
         <is>
           <t>car 3</t>
         </is>
       </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
-          <t>3 → 5</t>
+          <t>4 → 5</t>
         </is>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="Q6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="U6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="W6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="Y6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AA6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AE6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AG6" s="14" t="inlineStr">
-        <is>
-          <t>car 4</t>
+      <c r="AG6" s="12" t="inlineStr">
+        <is>
+          <t>dummy car</t>
         </is>
       </c>
       <c r="AH6" s="2" t="inlineStr">
         <is>
-          <t>3 → 8</t>
+          <t>4 → 6</t>
         </is>
       </c>
     </row>
     <row r="7" ht="50" customHeight="1">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="8" t="n">
         <v>48</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="n">
         <v>49</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -1066,10 +1019,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>51</v>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1077,59 +1035,79 @@
           <t>←</t>
         </is>
       </c>
-      <c r="I7" s="12" t="n">
+      <c r="I7" s="3" t="n">
         <v>52</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="K7" s="12" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="n">
         <v>53</v>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="M7" s="12" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="n">
         <v>54</v>
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="O7" s="12" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="n">
         <v>55</v>
       </c>
       <c r="P7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="Q7" s="12" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="Q7" s="3" t="n">
         <v>56</v>
       </c>
-      <c r="S7" s="12" t="n">
+      <c r="R7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="S7" s="3" t="n">
         <v>57</v>
       </c>
       <c r="T7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="U7" s="7" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="U7" s="6" t="n">
         <v>58</v>
       </c>
-      <c r="W7" s="7" t="n">
+      <c r="V7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="W7" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="Y7" s="3" t="n">
+      <c r="X7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="Y7" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="AA7" s="3" t="n">
+      <c r="Z7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AA7" s="6" t="n">
         <v>61</v>
       </c>
       <c r="AB7" s="2" t="inlineStr">
@@ -1137,7 +1115,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AC7" s="3" t="n">
+      <c r="AC7" s="6" t="n">
         <v>62</v>
       </c>
       <c r="AD7" s="2" t="inlineStr">
@@ -1145,32 +1123,11 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AE7" s="3" t="n">
+      <c r="AE7" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="AG7" s="15" t="inlineStr">
-        <is>
-          <t>car 5</t>
-        </is>
-      </c>
-      <c r="AH7" s="2" t="inlineStr">
-        <is>
-          <t>3 → 8</t>
-        </is>
-      </c>
     </row>
-    <row r="8" ht="20" customHeight="1">
-      <c r="AG8" s="16" t="inlineStr">
-        <is>
-          <t>dummy car</t>
-        </is>
-      </c>
-      <c r="AH8" s="2" t="inlineStr">
-        <is>
-          <t>3 → 9</t>
-        </is>
-      </c>
-    </row>
+    <row r="8" ht="20" customHeight="1"/>
     <row r="9" ht="50" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1183,7 +1140,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1230,6 +1187,11 @@
       <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
@@ -1254,10 +1216,15 @@
           <t>→</t>
         </is>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="I1" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="n">
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="n">
         <v>5</v>
       </c>
       <c r="L1" s="2" t="inlineStr">
@@ -1265,7 +1232,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="M1" s="4" t="n">
+      <c r="M1" s="3" t="n">
         <v>6</v>
       </c>
       <c r="N1" s="2" t="inlineStr">
@@ -1273,7 +1240,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="O1" s="4" t="n">
+      <c r="O1" s="3" t="n">
         <v>7</v>
       </c>
       <c r="P1" s="2" t="inlineStr">
@@ -1281,7 +1248,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="n">
+      <c r="Q1" s="4" t="n">
         <v>8</v>
       </c>
       <c r="R1" s="2" t="inlineStr">
@@ -1289,35 +1256,50 @@
           <t>←</t>
         </is>
       </c>
-      <c r="S1" s="6" t="n">
+      <c r="S1" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="U1" s="7" t="n">
+      <c r="U1" s="6" t="n">
         <v>10</v>
       </c>
       <c r="V1" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="W1" s="7" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="W1" s="6" t="n">
         <v>11</v>
       </c>
       <c r="X1" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="Y1" s="3" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="Y1" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="AA1" s="3" t="n">
+      <c r="Z1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AA1" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="AC1" s="3" t="n">
+      <c r="AB1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AC1" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="AE1" s="3" t="n">
+      <c r="AD1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AE1" s="6" t="n">
         <v>15</v>
       </c>
       <c r="AG1" s="2" t="inlineStr">
@@ -1332,97 +1314,77 @@
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AA2" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="Q2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="U2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AA2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AC2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AE2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AG2" s="8" t="inlineStr">
+      <c r="AG2" s="7" t="inlineStr">
         <is>
           <t>car 0</t>
         </is>
       </c>
       <c r="AH2" s="2" t="inlineStr">
         <is>
-          <t>0 → 5</t>
+          <t>3 → 5</t>
         </is>
       </c>
     </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="n">
         <v>19</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="I3" s="9" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="n">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="K3" s="4" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="n">
         <v>22</v>
       </c>
       <c r="N3" s="2" t="inlineStr">
@@ -1430,10 +1392,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="O3" s="4" t="n">
+      <c r="O3" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q3" s="7" t="n">
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="Q3" s="3" t="n">
         <v>24</v>
       </c>
       <c r="R3" s="2" t="inlineStr">
@@ -1441,7 +1408,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="S3" s="7" t="n">
+      <c r="S3" s="3" t="n">
         <v>25</v>
       </c>
       <c r="T3" s="2" t="inlineStr">
@@ -1449,10 +1416,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="W3" s="7" t="n">
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="W3" s="6" t="n">
         <v>27</v>
       </c>
       <c r="X3" s="2" t="inlineStr">
@@ -1460,10 +1432,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Y3" s="3" t="n">
+      <c r="Y3" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="AA3" s="3" t="n">
+      <c r="Z3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AA3" s="6" t="n">
         <v>29</v>
       </c>
       <c r="AB3" s="2" t="inlineStr">
@@ -1471,92 +1448,47 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AC3" s="3" t="n">
+      <c r="AC3" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="AE3" s="3" t="n">
+      <c r="AD3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AE3" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="AG3" s="10" t="inlineStr">
+      <c r="AG3" s="9" t="inlineStr">
         <is>
           <t>car 1</t>
         </is>
       </c>
       <c r="AH3" s="2" t="inlineStr">
         <is>
-          <t>1 → 6</t>
+          <t>0 → 9</t>
         </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="M4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="S4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="U4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="W4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AA4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AC4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AE4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AG4" s="11" t="inlineStr">
+      <c r="AG4" s="10" t="inlineStr">
         <is>
           <t>car 2</t>
         </is>
       </c>
       <c r="AH4" s="2" t="inlineStr">
         <is>
-          <t>4 → 6</t>
+          <t>0 → 7</t>
         </is>
       </c>
     </row>
     <row r="5" ht="50" customHeight="1">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="8" t="n">
         <v>32</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1564,32 +1496,47 @@
           <t>→</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="8" t="n">
         <v>33</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>34</v>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G5" s="9" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="n">
         <v>37</v>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="M5" s="12" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="n">
         <v>38</v>
       </c>
       <c r="N5" s="2" t="inlineStr">
@@ -1597,21 +1544,31 @@
           <t>←</t>
         </is>
       </c>
-      <c r="O5" s="12" t="n">
+      <c r="O5" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="Q5" s="3" t="n">
         <v>40</v>
       </c>
       <c r="R5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="S5" s="12" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="S5" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="U5" s="6" t="n">
         <v>42</v>
       </c>
       <c r="V5" s="2" t="inlineStr">
@@ -1619,7 +1576,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="W5" s="7" t="n">
+      <c r="W5" s="6" t="n">
         <v>43</v>
       </c>
       <c r="X5" s="2" t="inlineStr">
@@ -1627,7 +1584,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Y5" s="3" t="n">
+      <c r="Y5" s="6" t="n">
         <v>44</v>
       </c>
       <c r="Z5" s="2" t="inlineStr">
@@ -1635,10 +1592,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AA5" s="3" t="n">
+      <c r="AA5" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="AC5" s="3" t="n">
+      <c r="AB5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AC5" s="6" t="n">
         <v>46</v>
       </c>
       <c r="AD5" s="2" t="inlineStr">
@@ -1646,69 +1608,39 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AE5" s="3" t="n">
+      <c r="AE5" s="6" t="n">
         <v>47</v>
       </c>
-      <c r="AG5" s="13" t="inlineStr">
+      <c r="AG5" s="11" t="inlineStr">
         <is>
           <t>car 3</t>
         </is>
       </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
-          <t>3 → 5</t>
+          <t>4 → 5</t>
         </is>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AA6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AC6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AG6" s="14" t="inlineStr">
-        <is>
-          <t>car 4</t>
+      <c r="AG6" s="12" t="inlineStr">
+        <is>
+          <t>dummy car</t>
         </is>
       </c>
       <c r="AH6" s="2" t="inlineStr">
         <is>
-          <t>3 → 8</t>
+          <t>4 → 6</t>
         </is>
       </c>
     </row>
     <row r="7" ht="50" customHeight="1">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="8" t="n">
         <v>48</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1716,40 +1648,55 @@
           <t>→</t>
         </is>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="8" t="n">
         <v>49</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
         <v>50</v>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G7" s="9" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="I7" s="12" t="n">
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="K7" s="12" t="n">
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="n">
         <v>53</v>
       </c>
-      <c r="M7" s="12" t="n">
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="n">
         <v>54</v>
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="O7" s="12" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="O7" s="3" t="n">
         <v>55</v>
       </c>
       <c r="P7" s="2" t="inlineStr">
@@ -1757,7 +1704,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Q7" s="12" t="n">
+      <c r="Q7" s="3" t="n">
         <v>56</v>
       </c>
       <c r="R7" s="2" t="inlineStr">
@@ -1765,7 +1712,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="S7" s="12" t="n">
+      <c r="S7" s="3" t="n">
         <v>57</v>
       </c>
       <c r="T7" s="2" t="inlineStr">
@@ -1773,7 +1720,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="U7" s="7" t="n">
+      <c r="U7" s="6" t="n">
         <v>58</v>
       </c>
       <c r="V7" s="2" t="inlineStr">
@@ -1781,21 +1728,31 @@
           <t>←</t>
         </is>
       </c>
-      <c r="W7" s="7" t="n">
+      <c r="W7" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="Y7" s="3" t="n">
+      <c r="X7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="Y7" s="6" t="n">
         <v>60</v>
       </c>
       <c r="Z7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="AA7" s="3" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AA7" s="6" t="n">
         <v>61</v>
       </c>
-      <c r="AC7" s="3" t="n">
+      <c r="AB7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AC7" s="6" t="n">
         <v>62</v>
       </c>
       <c r="AD7" s="2" t="inlineStr">
@@ -1803,32 +1760,11 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AE7" s="3" t="n">
+      <c r="AE7" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="AG7" s="15" t="inlineStr">
-        <is>
-          <t>car 5</t>
-        </is>
-      </c>
-      <c r="AH7" s="2" t="inlineStr">
-        <is>
-          <t>3 → 8</t>
-        </is>
-      </c>
     </row>
-    <row r="8" ht="20" customHeight="1">
-      <c r="AG8" s="16" t="inlineStr">
-        <is>
-          <t>dummy car</t>
-        </is>
-      </c>
-      <c r="AH8" s="2" t="inlineStr">
-        <is>
-          <t>3 → 9</t>
-        </is>
-      </c>
-    </row>
+    <row r="8" ht="20" customHeight="1"/>
     <row r="9" ht="50" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add and fix new hold penalty
</commit_message>
<xml_diff>
--- a/results_Potential_NextBlock.xlsx
+++ b/results_Potential_NextBlock.xlsx
@@ -27,7 +27,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -36,12 +36,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="0087CEEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="000000FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
+        <fgColor rgb="00FFC0CB"/>
       </patternFill>
     </fill>
     <fill>
@@ -56,7 +66,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFC0CB"/>
+        <fgColor rgb="00FAEBD7"/>
       </patternFill>
     </fill>
   </fills>
@@ -100,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
@@ -117,25 +127,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -503,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,10 +585,15 @@
           <t>←</t>
         </is>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="E1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="n">
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="inlineStr">
@@ -574,20 +601,30 @@
           <t>←</t>
         </is>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="1" t="n">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="K1" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="M1" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="O1" s="3" t="n">
         <v>7</v>
       </c>
@@ -599,7 +636,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="S1" s="3" t="n">
+      <c r="S1" s="5" t="n">
         <v>9</v>
       </c>
       <c r="T1" s="2" t="inlineStr">
@@ -623,7 +660,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Y1" s="5" t="n">
+      <c r="Y1" s="6" t="n">
         <v>12</v>
       </c>
       <c r="Z1" s="2" t="inlineStr">
@@ -631,18 +668,23 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AA1" s="5" t="n">
+      <c r="AA1" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="AC1" s="5" t="n">
+      <c r="AB1" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AC1" s="7" t="n">
         <v>14</v>
       </c>
       <c r="AD1" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="AE1" s="5" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AE1" s="7" t="n">
         <v>15</v>
       </c>
       <c r="AG1" s="2" t="inlineStr">
@@ -653,58 +695,43 @@
       <c r="AH1" s="2" t="inlineStr">
         <is>
           <t>LP → DP</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="inlineStr">
+        <is>
+          <t>car amount (RT)</t>
         </is>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="E2" s="2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
       <c r="S2" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="W2" s="2" t="inlineStr">
+      <c r="AC2" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="AA2" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AE2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AG2" s="6" t="inlineStr">
+      <c r="AG2" s="8" t="inlineStr">
         <is>
           <t>car 0</t>
         </is>
       </c>
       <c r="AH2" s="2" t="inlineStr">
         <is>
-          <t>3 → 5</t>
+          <t>0 → 9</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>41 (RT)</t>
         </is>
       </c>
     </row>
@@ -725,7 +752,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="1" t="n">
         <v>18</v>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -733,7 +760,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="1" t="n">
         <v>19</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -741,7 +768,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="1" t="n">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="inlineStr">
@@ -754,12 +781,17 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="M3" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="O3" s="3" t="n">
         <v>23</v>
       </c>
@@ -776,7 +808,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="S3" s="3" t="n">
+      <c r="S3" s="5" t="n">
         <v>25</v>
       </c>
       <c r="T3" s="2" t="inlineStr">
@@ -787,21 +819,31 @@
       <c r="U3" s="5" t="n">
         <v>26</v>
       </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="W3" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="Y3" s="5" t="n">
+      <c r="X3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="Y3" s="9" t="n">
         <v>28</v>
       </c>
-      <c r="AA3" s="5" t="n">
+      <c r="Z3" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AA3" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="AB3" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="AC3" s="5" t="n">
+      <c r="AC3" s="7" t="n">
         <v>30</v>
       </c>
       <c r="AD3" s="2" t="inlineStr">
@@ -809,71 +851,86 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AE3" s="5" t="n">
+      <c r="AE3" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="AG3" s="7" t="inlineStr">
+      <c r="AG3" s="10" t="inlineStr">
         <is>
           <t>car 1</t>
         </is>
       </c>
       <c r="AH3" s="2" t="inlineStr">
         <is>
-          <t>0 → 9</t>
+          <t>0 → 7</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>61 (RT)</t>
         </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O4" s="2" t="inlineStr">
+      <c r="W4" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="Q4" s="2" t="inlineStr">
+      <c r="AC4" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="U4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="Y4" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AG4" s="8" t="inlineStr">
+      <c r="AG4" s="11" t="inlineStr">
         <is>
           <t>car 2</t>
         </is>
       </c>
       <c r="AH4" s="2" t="inlineStr">
         <is>
-          <t>0 → 7</t>
+          <t>4 → 5</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>114 (RT)</t>
         </is>
       </c>
     </row>
     <row r="5" ht="50" customHeight="1">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -892,12 +949,27 @@
       <c r="M5" s="3" t="n">
         <v>38</v>
       </c>
+      <c r="N5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="O5" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="Q5" s="3" t="n">
         <v>40</v>
       </c>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="S5" s="5" t="n">
         <v>41</v>
       </c>
@@ -911,7 +983,7 @@
       </c>
       <c r="V5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="W5" s="5" t="n">
@@ -922,103 +994,78 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Y5" s="5" t="n">
+      <c r="Y5" s="9" t="n">
         <v>44</v>
       </c>
-      <c r="Z5" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="AA5" s="5" t="n">
+      <c r="AA5" s="9" t="n">
         <v>45</v>
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="AC5" s="5" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AC5" s="7" t="n">
         <v>46</v>
       </c>
-      <c r="AE5" s="5" t="n">
+      <c r="AD5" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AE5" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="AG5" s="10" t="inlineStr">
+      <c r="AG5" s="12" t="inlineStr">
         <is>
           <t>car 3</t>
         </is>
       </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
-          <t>4 → 5</t>
+          <t>4 → 6</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>117 (RT)</t>
         </is>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="inlineStr">
+      <c r="K6" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="S6" s="2" t="inlineStr">
+      <c r="U6" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="U6" s="2" t="inlineStr">
+      <c r="AC6" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
       </c>
-      <c r="W6" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="AE6" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="AG6" s="11" t="inlineStr">
-        <is>
-          <t>dummy car</t>
+      <c r="AG6" s="13" t="inlineStr">
+        <is>
+          <t>car 4</t>
         </is>
       </c>
       <c r="AH6" s="2" t="inlineStr">
         <is>
-          <t>4 → 6</t>
+          <t>0 → 5</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>6 (RT)</t>
         </is>
       </c>
     </row>
     <row r="7" ht="50" customHeight="1">
-      <c r="A7" s="9" t="n">
+      <c r="A7" s="1" t="n">
         <v>48</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1026,7 +1073,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -1034,7 +1081,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="1" t="n">
         <v>50</v>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1042,7 +1089,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="1" t="n">
         <v>51</v>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1050,7 +1097,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="1" t="n">
         <v>52</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
@@ -1063,7 +1110,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="M7" s="3" t="n">
@@ -1071,7 +1118,7 @@
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="O7" s="3" t="n">
@@ -1082,15 +1129,25 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Q7" s="12" t="n">
+      <c r="Q7" s="14" t="n">
         <v>56</v>
       </c>
       <c r="S7" s="5" t="n">
         <v>57</v>
       </c>
+      <c r="T7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="U7" s="5" t="n">
         <v>58</v>
       </c>
+      <c r="V7" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="W7" s="5" t="n">
         <v>59</v>
       </c>
@@ -1099,7 +1156,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="Y7" s="5" t="n">
+      <c r="Y7" s="9" t="n">
         <v>60</v>
       </c>
       <c r="Z7" s="2" t="inlineStr">
@@ -1107,15 +1164,10 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AA7" s="5" t="n">
+      <c r="AA7" s="9" t="n">
         <v>61</v>
       </c>
-      <c r="AB7" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="AC7" s="5" t="n">
+      <c r="AC7" s="7" t="n">
         <v>62</v>
       </c>
       <c r="AD7" s="2" t="inlineStr">
@@ -1123,11 +1175,37 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AE7" s="5" t="n">
+      <c r="AE7" s="7" t="n">
         <v>63</v>
       </c>
+      <c r="AG7" s="15" t="inlineStr">
+        <is>
+          <t>car 5</t>
+        </is>
+      </c>
+      <c r="AH7" s="2" t="inlineStr">
+        <is>
+          <t>3 → 8</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>161 (RT)</t>
+        </is>
+      </c>
     </row>
-    <row r="8" ht="20" customHeight="1"/>
+    <row r="8" ht="20" customHeight="1">
+      <c r="AG8" s="16" t="inlineStr">
+        <is>
+          <t>dummy car</t>
+        </is>
+      </c>
+      <c r="AH8" s="2" t="inlineStr">
+        <is>
+          <t>0 → 6</t>
+        </is>
+      </c>
+    </row>
     <row r="9" ht="50" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1140,7 +1218,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1200,7 +1278,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="E1" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="inlineStr">
@@ -1208,7 +1286,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="G1" s="3" t="n">
+      <c r="G1" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="inlineStr">
@@ -1216,7 +1294,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="1" t="n">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="inlineStr">
@@ -1237,7 +1315,7 @@
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="O1" s="3" t="n">
@@ -1251,7 +1329,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="S1" s="3" t="n">
+      <c r="S1" s="5" t="n">
         <v>9</v>
       </c>
       <c r="T1" s="2" t="inlineStr">
@@ -1275,7 +1353,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Y1" s="5" t="n">
+      <c r="Y1" s="6" t="n">
         <v>12</v>
       </c>
       <c r="Z1" s="2" t="inlineStr">
@@ -1283,7 +1361,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AA1" s="5" t="n">
+      <c r="AA1" s="7" t="n">
         <v>13</v>
       </c>
       <c r="AB1" s="2" t="inlineStr">
@@ -1291,7 +1369,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AC1" s="5" t="n">
+      <c r="AC1" s="7" t="n">
         <v>14</v>
       </c>
       <c r="AD1" s="2" t="inlineStr">
@@ -1299,7 +1377,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AE1" s="5" t="n">
+      <c r="AE1" s="7" t="n">
         <v>15</v>
       </c>
       <c r="AG1" s="2" t="inlineStr">
@@ -1310,11 +1388,16 @@
       <c r="AH1" s="2" t="inlineStr">
         <is>
           <t>LP → DP</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="inlineStr">
+        <is>
+          <t>car amount (RT)</t>
         </is>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="O2" s="2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>↓</t>
         </is>
@@ -1324,14 +1407,24 @@
           <t>↑</t>
         </is>
       </c>
-      <c r="AG2" s="6" t="inlineStr">
+      <c r="AC2" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AG2" s="8" t="inlineStr">
         <is>
           <t>car 0</t>
         </is>
       </c>
       <c r="AH2" s="2" t="inlineStr">
         <is>
-          <t>3 → 5</t>
+          <t>0 → 9</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>41 (RT)</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1445,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="1" t="n">
         <v>18</v>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -1360,7 +1453,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="1" t="n">
         <v>19</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1368,7 +1461,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="1" t="n">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="inlineStr">
@@ -1408,7 +1501,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="S3" s="3" t="n">
+      <c r="S3" s="5" t="n">
         <v>25</v>
       </c>
       <c r="T3" s="2" t="inlineStr">
@@ -1427,28 +1520,23 @@
       <c r="W3" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="X3" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="Y3" s="5" t="n">
+      <c r="Y3" s="9" t="n">
         <v>28</v>
       </c>
       <c r="Z3" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="AA3" s="5" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AA3" s="7" t="n">
         <v>29</v>
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="AC3" s="5" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AC3" s="7" t="n">
         <v>30</v>
       </c>
       <c r="AD3" s="2" t="inlineStr">
@@ -1456,39 +1544,54 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AE3" s="5" t="n">
+      <c r="AE3" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="AG3" s="7" t="inlineStr">
+      <c r="AG3" s="10" t="inlineStr">
         <is>
           <t>car 1</t>
         </is>
       </c>
       <c r="AH3" s="2" t="inlineStr">
         <is>
-          <t>0 → 9</t>
+          <t>0 → 7</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>61 (RT)</t>
         </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="Q4" s="2" t="inlineStr">
+      <c r="W4" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="AG4" s="8" t="inlineStr">
+      <c r="AC4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AG4" s="11" t="inlineStr">
         <is>
           <t>car 2</t>
         </is>
       </c>
       <c r="AH4" s="2" t="inlineStr">
         <is>
-          <t>0 → 7</t>
+          <t>4 → 5</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>114 (RT)</t>
         </is>
       </c>
     </row>
     <row r="5" ht="50" customHeight="1">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1496,7 +1599,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="1" t="n">
         <v>33</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -1504,7 +1607,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="1" t="n">
         <v>34</v>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -1512,7 +1615,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="1" t="n">
         <v>35</v>
       </c>
       <c r="H5" s="2" t="inlineStr">
@@ -1520,7 +1623,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="1" t="n">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -1557,7 +1660,7 @@
       </c>
       <c r="R5" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="S5" s="5" t="n">
@@ -1565,7 +1668,7 @@
       </c>
       <c r="T5" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="U5" s="5" t="n">
@@ -1573,7 +1676,7 @@
       </c>
       <c r="V5" s="2" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="W5" s="5" t="n">
@@ -1584,23 +1687,18 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Y5" s="5" t="n">
+      <c r="Y5" s="9" t="n">
         <v>44</v>
       </c>
-      <c r="Z5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="AA5" s="5" t="n">
+      <c r="AA5" s="9" t="n">
         <v>45</v>
       </c>
       <c r="AB5" s="2" t="inlineStr">
         <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="AC5" s="5" t="n">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="AC5" s="7" t="n">
         <v>46</v>
       </c>
       <c r="AD5" s="2" t="inlineStr">
@@ -1608,44 +1706,59 @@
           <t>←</t>
         </is>
       </c>
-      <c r="AE5" s="5" t="n">
+      <c r="AE5" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="AG5" s="10" t="inlineStr">
+      <c r="AG5" s="12" t="inlineStr">
         <is>
           <t>car 3</t>
         </is>
       </c>
       <c r="AH5" s="2" t="inlineStr">
         <is>
-          <t>4 → 5</t>
+          <t>4 → 6</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>117 (RT)</t>
         </is>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="O6" s="2" t="inlineStr">
+      <c r="K6" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="AE6" s="2" t="inlineStr">
+      <c r="U6" s="2" t="inlineStr">
         <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="AG6" s="11" t="inlineStr">
-        <is>
-          <t>dummy car</t>
+      <c r="AC6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AG6" s="13" t="inlineStr">
+        <is>
+          <t>car 4</t>
         </is>
       </c>
       <c r="AH6" s="2" t="inlineStr">
         <is>
-          <t>4 → 6</t>
+          <t>0 → 5</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>6 (RT)</t>
         </is>
       </c>
     </row>
     <row r="7" ht="50" customHeight="1">
-      <c r="A7" s="9" t="n">
+      <c r="A7" s="1" t="n">
         <v>48</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1653,7 +1766,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -1661,7 +1774,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="1" t="n">
         <v>50</v>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -1669,7 +1782,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="1" t="n">
         <v>51</v>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1677,7 +1790,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="1" t="n">
         <v>52</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
@@ -1690,7 +1803,7 @@
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="M7" s="3" t="n">
@@ -1698,7 +1811,7 @@
       </c>
       <c r="N7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="O7" s="3" t="n">
@@ -1709,7 +1822,7 @@
           <t>←</t>
         </is>
       </c>
-      <c r="Q7" s="12" t="n">
+      <c r="Q7" s="14" t="n">
         <v>56</v>
       </c>
       <c r="S7" s="5" t="n">
@@ -1725,18 +1838,13 @@
       </c>
       <c r="V7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="W7" s="5" t="n">
         <v>59</v>
       </c>
-      <c r="X7" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="Y7" s="5" t="n">
+      <c r="Y7" s="9" t="n">
         <v>60</v>
       </c>
       <c r="Z7" s="2" t="inlineStr">
@@ -1744,7 +1852,7 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AA7" s="5" t="n">
+      <c r="AA7" s="9" t="n">
         <v>61</v>
       </c>
       <c r="AB7" s="2" t="inlineStr">
@@ -1752,19 +1860,45 @@
           <t>→</t>
         </is>
       </c>
-      <c r="AC7" s="5" t="n">
+      <c r="AC7" s="7" t="n">
         <v>62</v>
       </c>
       <c r="AD7" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="AE7" s="5" t="n">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AE7" s="7" t="n">
         <v>63</v>
       </c>
+      <c r="AG7" s="15" t="inlineStr">
+        <is>
+          <t>car 5</t>
+        </is>
+      </c>
+      <c r="AH7" s="2" t="inlineStr">
+        <is>
+          <t>3 → 8</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>161 (RT)</t>
+        </is>
+      </c>
     </row>
-    <row r="8" ht="20" customHeight="1"/>
+    <row r="8" ht="20" customHeight="1">
+      <c r="AG8" s="16" t="inlineStr">
+        <is>
+          <t>dummy car</t>
+        </is>
+      </c>
+      <c r="AH8" s="2" t="inlineStr">
+        <is>
+          <t>0 → 6</t>
+        </is>
+      </c>
+    </row>
     <row r="9" ht="50" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>